<commit_message>
Nuevos partidos - apuestas del 31/05
</commit_message>
<xml_diff>
--- a/Otras cosas/Apuestas.xlsx
+++ b/Otras cosas/Apuestas.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Kike\Otros_RepositorioGit\Otras cosas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA315FEC-4B73-494A-B4EE-904FAB93D4F3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="MAYO_2018" sheetId="4" r:id="rId1"/>
     <sheet name="Hoja vacía_02" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="73">
   <si>
     <t>Cuota</t>
   </si>
@@ -228,13 +222,34 @@
   </si>
   <si>
     <t>Cuota media -&gt;&gt;</t>
+  </si>
+  <si>
+    <t>PUSH</t>
+  </si>
+  <si>
+    <t>Islandia</t>
+  </si>
+  <si>
+    <t>Handicap asiático</t>
+  </si>
+  <si>
+    <t>Kopavogur - Leiknir : Kopavogur -1.0</t>
+  </si>
+  <si>
+    <t>Flamengo - Bahia : Flamengo -1</t>
+  </si>
+  <si>
+    <t>Paranaense - Santos : NO</t>
+  </si>
+  <si>
+    <t>Paranaense - Santos : Paranaense</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +277,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -683,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -831,6 +852,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,7 +925,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -924,27 +957,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -976,24 +991,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1169,14 +1166,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="57.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
@@ -1186,8 +1183,8 @@
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:13">
       <c r="B2" t="s">
         <v>45</v>
       </c>
@@ -1197,7 +1194,7 @@
       <c r="E2" s="51"/>
       <c r="F2" s="40">
         <f>SUM(J:J)</f>
-        <v>5.9424999999999999</v>
+        <v>7.1924999999999999</v>
       </c>
       <c r="G2" s="42" t="s">
         <v>2</v>
@@ -1207,24 +1204,24 @@
       </c>
       <c r="I2" s="2">
         <f>COUNTIF(B:B,"YES")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
         <v>64</v>
       </c>
       <c r="M2">
         <f>SUM(E6:E150)/COUNT(E6:E150)</f>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.3214285714285714</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="15.75" thickBot="1">
       <c r="D3" s="52" t="s">
         <v>39</v>
       </c>
       <c r="E3" s="53"/>
       <c r="F3" s="41">
         <f>SUM(J:J)/SUM(E:E)*100</f>
-        <v>18.5703125</v>
+        <v>19.439189189189186</v>
       </c>
       <c r="G3" s="43" t="s">
         <v>40</v>
@@ -1241,11 +1238,11 @@
       </c>
       <c r="M3">
         <f>SUM(D6:D150)/COUNT(D6:D150)</f>
-        <v>2.0293478260869562</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0361111111111105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:13" ht="15.75" thickBot="1">
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1274,7 +1271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13">
       <c r="B6" s="18" t="s">
         <v>5</v>
       </c>
@@ -1304,7 +1301,7 @@
         <v>1.3499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13">
       <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
@@ -1334,7 +1331,7 @@
         <v>-1.25</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="30">
       <c r="B8" s="24" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1361,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="30">
       <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
@@ -1394,7 +1391,7 @@
         <v>2.0999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="30">
       <c r="B10" s="24" t="s">
         <v>5</v>
       </c>
@@ -1424,7 +1421,7 @@
         <v>1.0375000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="33" customHeight="1">
       <c r="B11" s="22" t="s">
         <v>6</v>
       </c>
@@ -1454,7 +1451,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="30">
       <c r="B12" s="22" t="s">
         <v>6</v>
       </c>
@@ -1484,7 +1481,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="30">
       <c r="B13" s="22" t="s">
         <v>6</v>
       </c>
@@ -1514,7 +1511,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="30">
       <c r="B14" s="24" t="s">
         <v>5</v>
       </c>
@@ -1544,7 +1541,7 @@
         <v>0.99000000000000021</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="30">
       <c r="B15" s="24" t="s">
         <v>5</v>
       </c>
@@ -1574,7 +1571,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="30">
       <c r="B16" s="22" t="s">
         <v>6</v>
       </c>
@@ -1604,7 +1601,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="B17" s="22" t="s">
         <v>6</v>
       </c>
@@ -1634,7 +1631,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10">
       <c r="B18" s="24" t="s">
         <v>5</v>
       </c>
@@ -1664,7 +1661,7 @@
         <v>0.39999999999999991</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10">
       <c r="B19" s="24" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +1691,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10">
       <c r="B20" s="22" t="s">
         <v>6</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10">
       <c r="B21" s="22" t="s">
         <v>6</v>
       </c>
@@ -1754,7 +1751,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10">
       <c r="B22" s="24" t="s">
         <v>5</v>
       </c>
@@ -1784,7 +1781,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10">
       <c r="B23" s="24" t="s">
         <v>5</v>
       </c>
@@ -1814,7 +1811,7 @@
         <v>0.65999999999999992</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10">
       <c r="B24" s="24" t="s">
         <v>5</v>
       </c>
@@ -1844,7 +1841,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10">
       <c r="B25" s="22" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +1871,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10">
       <c r="B26" s="24" t="s">
         <v>5</v>
       </c>
@@ -1904,7 +1901,7 @@
         <v>2.1399999999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10">
       <c r="B27" s="24" t="s">
         <v>5</v>
       </c>
@@ -1934,7 +1931,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10">
       <c r="B28" s="24" t="s">
         <v>5</v>
       </c>
@@ -1964,7 +1961,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10">
       <c r="B29" s="24" t="s">
         <v>5</v>
       </c>
@@ -1994,63 +1991,123 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="27">
+    <row r="30" spans="2:10">
+      <c r="B30" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="56">
+        <v>1.9</v>
+      </c>
+      <c r="E30" s="56">
+        <v>2</v>
+      </c>
+      <c r="F30" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" s="57">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="45"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="27">
+    <row r="31" spans="2:10">
+      <c r="B31" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="49">
+        <v>2.25</v>
+      </c>
+      <c r="E31" s="49">
+        <v>1</v>
+      </c>
+      <c r="F31" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
       <c r="B32" s="45"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
+      <c r="C32" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="47">
+        <v>1.9</v>
+      </c>
+      <c r="E32" s="47">
+        <v>1</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="J32" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10">
       <c r="B33" s="45"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
+      <c r="C33" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="47">
+        <v>2.25</v>
+      </c>
+      <c r="E33" s="47">
+        <v>1</v>
+      </c>
+      <c r="F33" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="47" t="s">
+        <v>60</v>
+      </c>
       <c r="J33" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10">
       <c r="B34" s="45"/>
       <c r="C34" s="46"/>
       <c r="D34" s="47"/>
@@ -2064,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="15.75" thickBot="1">
       <c r="B35" s="28"/>
       <c r="C35" s="29"/>
       <c r="D35" s="30"/>
@@ -2078,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10">
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
       <c r="D36" s="13"/>
@@ -2099,14 +2156,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1"/>
@@ -2119,8 +2176,8 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:10">
       <c r="D2" s="50" t="s">
         <v>7</v>
       </c>
@@ -2140,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
       <c r="D3" s="52" t="s">
         <v>39</v>
       </c>
@@ -2160,8 +2217,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:10" ht="15.75" thickBot="1">
       <c r="B5" s="36" t="s">
         <v>9</v>
       </c>
@@ -2190,7 +2247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" s="32"/>
       <c r="C6" s="33"/>
       <c r="D6" s="34"/>
@@ -2204,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" s="26"/>
       <c r="C7" s="15"/>
       <c r="D7" s="10"/>
@@ -2218,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" s="26"/>
       <c r="C8" s="15"/>
       <c r="D8" s="10"/>
@@ -2232,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" s="26"/>
       <c r="C9" s="15"/>
       <c r="D9" s="10"/>
@@ -2246,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" s="26"/>
       <c r="C10" s="15"/>
       <c r="D10" s="10"/>
@@ -2260,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" s="26"/>
       <c r="C11" s="15"/>
       <c r="D11" s="10"/>
@@ -2274,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" s="26"/>
       <c r="C12" s="15"/>
       <c r="D12" s="10"/>
@@ -2288,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" s="26"/>
       <c r="C13" s="15"/>
       <c r="D13" s="10"/>
@@ -2302,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10">
       <c r="B14" s="26"/>
       <c r="C14" s="15"/>
       <c r="D14" s="10"/>
@@ -2316,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" s="26"/>
       <c r="C15" s="15"/>
       <c r="D15" s="10"/>
@@ -2330,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" s="26"/>
       <c r="C16" s="15"/>
       <c r="D16" s="10"/>
@@ -2344,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="B17" s="26"/>
       <c r="C17" s="15"/>
       <c r="D17" s="10"/>
@@ -2358,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10">
       <c r="B18" s="26"/>
       <c r="C18" s="15"/>
       <c r="D18" s="10"/>
@@ -2372,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10">
       <c r="B19" s="26"/>
       <c r="C19" s="15"/>
       <c r="D19" s="10"/>
@@ -2386,7 +2443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10">
       <c r="B20" s="26"/>
       <c r="C20" s="15"/>
       <c r="D20" s="10"/>
@@ -2400,7 +2457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10">
       <c r="B21" s="26"/>
       <c r="C21" s="15"/>
       <c r="D21" s="10"/>
@@ -2414,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10">
       <c r="B22" s="26"/>
       <c r="C22" s="15"/>
       <c r="D22" s="10"/>
@@ -2428,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="15.75" thickBot="1">
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
       <c r="D23" s="30"/>

</xml_diff>

<commit_message>
Mes de MAYO terminado - Comenzamos JUNIO
</commit_message>
<xml_diff>
--- a/Otras cosas/Apuestas.xlsx
+++ b/Otras cosas/Apuestas.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Kike\Otros_RepositorioGit\Otras cosas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEA4702-A2F9-4636-82F2-509C3117C966}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAYO_2018" sheetId="4" r:id="rId1"/>
-    <sheet name="Hoja vacía_02" sheetId="5" r:id="rId2"/>
+    <sheet name="JUNIO_2018" sheetId="6" r:id="rId2"/>
+    <sheet name="BOCETO" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="76">
   <si>
     <t>Cuota</t>
   </si>
@@ -243,15 +250,40 @@
   </si>
   <si>
     <t>Paranaense - Santos : Paranaense</t>
+  </si>
+  <si>
+    <t>TERMINAMOS MAYO CON</t>
+  </si>
+  <si>
+    <t>UNIDADES</t>
+  </si>
+  <si>
+    <t>TERMINAMOS EL MES CON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -284,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -700,11 +732,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -841,6 +935,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -853,17 +959,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,7 +1034,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -957,9 +1066,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -991,6 +1118,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1166,14 +1311,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:M36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="57.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
@@ -1183,18 +1326,18 @@
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:13">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="51"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="40">
         <f>SUM(J:J)</f>
-        <v>7.1924999999999999</v>
+        <v>9.3424999999999994</v>
       </c>
       <c r="G2" s="42" t="s">
         <v>2</v>
@@ -1204,24 +1347,25 @@
       </c>
       <c r="I2" s="2">
         <f>COUNTIF(B:B,"YES")</f>
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="M2">
+      <c r="L2" s="59"/>
+      <c r="M2" s="60">
         <f>SUM(E6:E150)/COUNT(E6:E150)</f>
         <v>1.3214285714285714</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="15.75" thickBot="1">
-      <c r="D3" s="52" t="s">
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="53"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="41">
         <f>SUM(J:J)/SUM(E:E)*100</f>
-        <v>19.439189189189186</v>
+        <v>25.25</v>
       </c>
       <c r="G3" s="43" t="s">
         <v>40</v>
@@ -1233,16 +1377,17 @@
         <f>COUNTIF(B:B,"NO")</f>
         <v>9</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="M3">
+      <c r="L3" s="62"/>
+      <c r="M3" s="63">
         <f>SUM(D6:D150)/COUNT(D6:D150)</f>
         <v>2.0361111111111105</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="15.75" thickBot="1"/>
-    <row r="5" spans="2:13" ht="15.75" thickBot="1">
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1271,7 +1416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>5</v>
       </c>
@@ -1301,7 +1446,7 @@
         <v>1.3499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
@@ -1330,8 +1475,14 @@
         <f>IF(B7="YES",SUM(D7-1)*E7,IF(B7="NO",-E7,0))</f>
         <v>-1.25</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" ht="30">
+      <c r="M7" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
+    </row>
+    <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>5</v>
       </c>
@@ -1360,8 +1511,12 @@
         <f t="shared" ref="J8:J15" si="0">IF(B8="YES",SUM(D8-1)*E8,IF(B8="NO",-E8,0))</f>
         <v>1.2000000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" ht="30">
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="64"/>
+    </row>
+    <row r="9" spans="2:16" ht="30" x14ac:dyDescent="0.45">
       <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
@@ -1390,8 +1545,17 @@
         <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" ht="30">
+      <c r="M9" s="66">
+        <f>F2</f>
+        <v>9.3424999999999994</v>
+      </c>
+      <c r="N9" s="66"/>
+      <c r="O9" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="65"/>
+    </row>
+    <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="24" t="s">
         <v>5</v>
       </c>
@@ -1421,7 +1585,7 @@
         <v>1.0375000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="33" customHeight="1">
+    <row r="11" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>6</v>
       </c>
@@ -1451,7 +1615,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="30">
+    <row r="12" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
         <v>6</v>
       </c>
@@ -1481,7 +1645,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="30">
+    <row r="13" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
         <v>6</v>
       </c>
@@ -1511,7 +1675,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="30">
+    <row r="14" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="24" t="s">
         <v>5</v>
       </c>
@@ -1541,7 +1705,7 @@
         <v>0.99000000000000021</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="30">
+    <row r="15" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
         <v>5</v>
       </c>
@@ -1571,7 +1735,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="30">
+    <row r="16" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
         <v>6</v>
       </c>
@@ -1601,7 +1765,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
         <v>6</v>
       </c>
@@ -1631,7 +1795,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
         <v>5</v>
       </c>
@@ -1661,7 +1825,7 @@
         <v>0.39999999999999991</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
         <v>5</v>
       </c>
@@ -1691,7 +1855,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>6</v>
       </c>
@@ -1721,7 +1885,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
         <v>6</v>
       </c>
@@ -1751,7 +1915,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="24" t="s">
         <v>5</v>
       </c>
@@ -1781,7 +1945,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
         <v>5</v>
       </c>
@@ -1811,7 +1975,7 @@
         <v>0.65999999999999992</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
         <v>5</v>
       </c>
@@ -1841,7 +2005,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
         <v>6</v>
       </c>
@@ -1871,7 +2035,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="24" t="s">
         <v>5</v>
       </c>
@@ -1901,7 +2065,7 @@
         <v>2.1399999999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="24" t="s">
         <v>5</v>
       </c>
@@ -1931,7 +2095,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="28" spans="2:10">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="24" t="s">
         <v>5</v>
       </c>
@@ -1961,7 +2125,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="24" t="s">
         <v>5</v>
       </c>
@@ -1991,37 +2155,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:10">
-      <c r="B30" s="54" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="55" t="s">
+      <c r="C30" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="56">
+      <c r="D30" s="52">
         <v>1.9</v>
       </c>
-      <c r="E30" s="56">
+      <c r="E30" s="52">
         <v>2</v>
       </c>
-      <c r="F30" s="56" t="s">
+      <c r="F30" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="56" t="s">
+      <c r="G30" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="56" t="s">
+      <c r="H30" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="56" t="s">
+      <c r="I30" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="J30" s="57">
+      <c r="J30" s="53">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
         <v>5</v>
       </c>
@@ -2051,63 +2215,67 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="45"/>
-      <c r="C32" s="46" t="s">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="47">
+      <c r="D32" s="49">
         <v>1.9</v>
       </c>
-      <c r="E32" s="47">
+      <c r="E32" s="49">
         <v>1</v>
       </c>
-      <c r="F32" s="47" t="s">
+      <c r="F32" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="47" t="s">
+      <c r="G32" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="47" t="s">
+      <c r="H32" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="47" t="s">
+      <c r="I32" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="J32" s="27">
+      <c r="J32" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10">
-      <c r="B33" s="45"/>
-      <c r="C33" s="46" t="s">
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="47">
+      <c r="D33" s="49">
         <v>2.25</v>
       </c>
-      <c r="E33" s="47">
+      <c r="E33" s="49">
         <v>1</v>
       </c>
-      <c r="F33" s="47" t="s">
+      <c r="F33" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="47" t="s">
+      <c r="G33" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="H33" s="47" t="s">
+      <c r="H33" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="47" t="s">
+      <c r="I33" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="J33" s="27">
+      <c r="J33" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="45"/>
       <c r="C34" s="46"/>
       <c r="D34" s="47"/>
@@ -2121,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15.75" thickBot="1">
+    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="28"/>
       <c r="C35" s="29"/>
       <c r="D35" s="30"/>
@@ -2135,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:10">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
       <c r="D36" s="13"/>
@@ -2147,23 +2315,27 @@
       <c r="J36" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733C2A37-09AA-41E6-B976-502F90A9005E}">
+  <dimension ref="B1:P23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1"/>
@@ -2174,14 +2346,15 @@
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10">
-      <c r="D2" s="50" t="s">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="51"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="40">
         <f>SUM(J:J)</f>
         <v>0</v>
@@ -2196,12 +2369,20 @@
         <f>COUNTIF(B:B,"YES")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1">
-      <c r="D3" s="52" t="s">
+      <c r="K2" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="59"/>
+      <c r="M2" s="60" t="e">
+        <f>SUM(E6:E150)/COUNT(E6:E150)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="53"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="41" t="e">
         <f>SUM(J:J)/SUM(E:E)*100</f>
         <v>#DIV/0!</v>
@@ -2216,9 +2397,17 @@
         <f>COUNTIF(B:B,"NO")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1">
+      <c r="K3" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63" t="e">
+        <f>SUM(D6:D150)/COUNT(D6:D150)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="36" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="32"/>
       <c r="C6" s="33"/>
       <c r="D6" s="34"/>
@@ -2261,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="26"/>
       <c r="C7" s="15"/>
       <c r="D7" s="10"/>
@@ -2274,8 +2463,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:10">
+      <c r="M7" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
       <c r="C8" s="15"/>
       <c r="D8" s="10"/>
@@ -2288,8 +2483,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:10">
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="64"/>
+    </row>
+    <row r="9" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B9" s="26"/>
       <c r="C9" s="15"/>
       <c r="D9" s="10"/>
@@ -2302,8 +2501,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:10">
+      <c r="M9" s="66">
+        <f>F2</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="66"/>
+      <c r="O9" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="65"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="C10" s="15"/>
       <c r="D10" s="10"/>
@@ -2317,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>
       <c r="C11" s="15"/>
       <c r="D11" s="10"/>
@@ -2331,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="26"/>
       <c r="C12" s="15"/>
       <c r="D12" s="10"/>
@@ -2345,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="26"/>
       <c r="C13" s="15"/>
       <c r="D13" s="10"/>
@@ -2359,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="26"/>
       <c r="C14" s="15"/>
       <c r="D14" s="10"/>
@@ -2373,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="26"/>
       <c r="C15" s="15"/>
       <c r="D15" s="10"/>
@@ -2387,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="26"/>
       <c r="C16" s="15"/>
       <c r="D16" s="10"/>
@@ -2401,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="26"/>
       <c r="C17" s="15"/>
       <c r="D17" s="10"/>
@@ -2415,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="26"/>
       <c r="C18" s="15"/>
       <c r="D18" s="10"/>
@@ -2429,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="26"/>
       <c r="C19" s="15"/>
       <c r="D19" s="10"/>
@@ -2443,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="26"/>
       <c r="C20" s="15"/>
       <c r="D20" s="10"/>
@@ -2457,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="26"/>
       <c r="C21" s="15"/>
       <c r="D21" s="10"/>
@@ -2471,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="26"/>
       <c r="C22" s="15"/>
       <c r="D22" s="10"/>
@@ -2485,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15.75" thickBot="1">
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
       <c r="D23" s="30"/>
@@ -2500,9 +2708,404 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:P23"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D2" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="55"/>
+      <c r="F2" s="40">
+        <f>SUM(J:J)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="2">
+        <f>COUNTIF(B:B,"YES")</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="59"/>
+      <c r="M2" s="60" t="e">
+        <f>SUM(E6:E150)/COUNT(E6:E150)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="57"/>
+      <c r="F3" s="41" t="e">
+        <f>SUM(J:J)/SUM(E:E)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="4">
+        <f>COUNTIF(B:B,"NO")</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63" t="e">
+        <f>SUM(D6:D150)/COUNT(D6:D150)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="35">
+        <f t="shared" ref="J6:J16" si="0">IF(B6="YES",SUM(D6-1)*E6,IF(B6="NO",-E6,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="26"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="26"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="64"/>
+    </row>
+    <row r="9" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B9" s="26"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="66">
+        <f>F2</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="66"/>
+      <c r="O9" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="65"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="26"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="26"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="26"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="26"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="27">
+        <f t="shared" ref="J17:J23" si="1">IF(B17="YES",SUM(D17-1)*E17,IF(B17="NO",-E17,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="26"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="26"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="26"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="26"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Todo lo del fin de semana
</commit_message>
<xml_diff>
--- a/Otras cosas/Apuestas.xlsx
+++ b/Otras cosas/Apuestas.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Kike\Otros_RepositorioGit\Otras cosas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEA4702-A2F9-4636-82F2-509C3117C966}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="8130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAYO_2018" sheetId="4" r:id="rId1"/>
     <sheet name="JUNIO_2018" sheetId="6" r:id="rId2"/>
     <sheet name="BOCETO" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="98">
   <si>
     <t>Cuota</t>
   </si>
@@ -259,13 +253,79 @@
   </si>
   <si>
     <t>TERMINAMOS EL MES CON</t>
+  </si>
+  <si>
+    <t>Juventude vs Guarani : Sí</t>
+  </si>
+  <si>
+    <t>Segunda</t>
+  </si>
+  <si>
+    <t>Juventude vs Guarani : OVER 2.5</t>
+  </si>
+  <si>
+    <t>OVER/UNDER</t>
+  </si>
+  <si>
+    <t>Paysandu vs Boa : UNDER 2.5</t>
+  </si>
+  <si>
+    <t>Vila Nova vs CSA : UNDER 2.5</t>
+  </si>
+  <si>
+    <t>Hungría</t>
+  </si>
+  <si>
+    <t>Primera</t>
+  </si>
+  <si>
+    <t>Diosgyori VTK vs Videoton : OVER 2.5</t>
+  </si>
+  <si>
+    <t>Diosgyori VTK vs Videoton : Videoton o empate</t>
+  </si>
+  <si>
+    <t>Doble oportunidad</t>
+  </si>
+  <si>
+    <t>Balmazujvarosi vs Ferencvarosi : Ferencvarosi o empate</t>
+  </si>
+  <si>
+    <t>Balmazujvarosi vs Ferencvarosi : UNDER 2.5</t>
+  </si>
+  <si>
+    <t>Concordia vs Timisoara : UNDER 2.5</t>
+  </si>
+  <si>
+    <t>Rumanía</t>
+  </si>
+  <si>
+    <t>Concordia vs Timisoara : NO</t>
+  </si>
+  <si>
+    <t>Montreal Impact vs Dynamo : Dynamo o empate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEUU </t>
+  </si>
+  <si>
+    <t>MLS</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Columbus Crew vs Toronto : Columbus</t>
+  </si>
+  <si>
+    <t>Mineros vs Carabobo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,7 +376,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -794,11 +854,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -947,32 +1020,80 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1034,7 +1155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1066,27 +1187,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1118,24 +1221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1311,12 +1396,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="57.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
@@ -1326,15 +1411,15 @@
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:16">
       <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="55"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="40">
         <f>SUM(J:J)</f>
         <v>9.3424999999999994</v>
@@ -1349,20 +1434,20 @@
         <f>COUNTIF(B:B,"YES")</f>
         <v>18</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="60">
+      <c r="L2" s="55"/>
+      <c r="M2" s="56">
         <f>SUM(E6:E150)/COUNT(E6:E150)</f>
         <v>1.3214285714285714</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="56" t="s">
+    <row r="3" spans="2:16" ht="15.75" thickBot="1">
+      <c r="D3" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="57"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="41">
         <f>SUM(J:J)/SUM(E:E)*100</f>
         <v>25.25</v>
@@ -1377,17 +1462,17 @@
         <f>COUNTIF(B:B,"NO")</f>
         <v>9</v>
       </c>
-      <c r="K3" s="61" t="s">
+      <c r="K3" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63">
+      <c r="L3" s="58"/>
+      <c r="M3" s="59">
         <f>SUM(D6:D150)/COUNT(D6:D150)</f>
         <v>2.0361111111111105</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1">
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1416,7 +1501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16">
       <c r="B6" s="18" t="s">
         <v>5</v>
       </c>
@@ -1446,7 +1531,7 @@
         <v>1.3499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16">
       <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
@@ -1475,14 +1560,14 @@
         <f>IF(B7="YES",SUM(D7-1)*E7,IF(B7="NO",-E7,0))</f>
         <v>-1.25</v>
       </c>
-      <c r="M7" s="64" t="s">
+      <c r="M7" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-    </row>
-    <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+    </row>
+    <row r="8" spans="2:16" ht="30">
       <c r="B8" s="24" t="s">
         <v>5</v>
       </c>
@@ -1511,12 +1596,12 @@
         <f t="shared" ref="J8:J15" si="0">IF(B8="YES",SUM(D8-1)*E8,IF(B8="NO",-E8,0))</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-    </row>
-    <row r="9" spans="2:16" ht="30" x14ac:dyDescent="0.45">
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+    </row>
+    <row r="9" spans="2:16" ht="30">
       <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
@@ -1545,17 +1630,17 @@
         <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
-      <c r="M9" s="66">
+      <c r="M9" s="69">
         <f>F2</f>
         <v>9.3424999999999994</v>
       </c>
-      <c r="N9" s="66"/>
-      <c r="O9" s="65" t="s">
+      <c r="N9" s="69"/>
+      <c r="O9" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="P9" s="65"/>
-    </row>
-    <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="P9" s="70"/>
+    </row>
+    <row r="10" spans="2:16" ht="30">
       <c r="B10" s="24" t="s">
         <v>5</v>
       </c>
@@ -1585,7 +1670,7 @@
         <v>1.0375000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" ht="33" customHeight="1">
       <c r="B11" s="22" t="s">
         <v>6</v>
       </c>
@@ -1615,7 +1700,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="30">
       <c r="B12" s="22" t="s">
         <v>6</v>
       </c>
@@ -1645,7 +1730,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" ht="30">
       <c r="B13" s="22" t="s">
         <v>6</v>
       </c>
@@ -1675,7 +1760,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="30">
       <c r="B14" s="24" t="s">
         <v>5</v>
       </c>
@@ -1705,7 +1790,7 @@
         <v>0.99000000000000021</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="30">
       <c r="B15" s="24" t="s">
         <v>5</v>
       </c>
@@ -1735,7 +1820,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="30">
       <c r="B16" s="22" t="s">
         <v>6</v>
       </c>
@@ -1765,7 +1850,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="B17" s="22" t="s">
         <v>6</v>
       </c>
@@ -1795,7 +1880,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10">
       <c r="B18" s="24" t="s">
         <v>5</v>
       </c>
@@ -1825,7 +1910,7 @@
         <v>0.39999999999999991</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10">
       <c r="B19" s="24" t="s">
         <v>5</v>
       </c>
@@ -1855,7 +1940,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10">
       <c r="B20" s="22" t="s">
         <v>6</v>
       </c>
@@ -1885,7 +1970,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10">
       <c r="B21" s="22" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +2000,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10">
       <c r="B22" s="24" t="s">
         <v>5</v>
       </c>
@@ -1945,7 +2030,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10">
       <c r="B23" s="24" t="s">
         <v>5</v>
       </c>
@@ -1975,7 +2060,7 @@
         <v>0.65999999999999992</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10">
       <c r="B24" s="24" t="s">
         <v>5</v>
       </c>
@@ -2005,7 +2090,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10">
       <c r="B25" s="22" t="s">
         <v>6</v>
       </c>
@@ -2035,7 +2120,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10">
       <c r="B26" s="24" t="s">
         <v>5</v>
       </c>
@@ -2065,7 +2150,7 @@
         <v>2.1399999999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10">
       <c r="B27" s="24" t="s">
         <v>5</v>
       </c>
@@ -2095,7 +2180,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10">
       <c r="B28" s="24" t="s">
         <v>5</v>
       </c>
@@ -2125,7 +2210,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10">
       <c r="B29" s="24" t="s">
         <v>5</v>
       </c>
@@ -2155,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10">
       <c r="B30" s="50" t="s">
         <v>66</v>
       </c>
@@ -2185,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10">
       <c r="B31" s="24" t="s">
         <v>5</v>
       </c>
@@ -2215,7 +2300,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10">
       <c r="B32" s="24" t="s">
         <v>5</v>
       </c>
@@ -2245,7 +2330,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10">
       <c r="B33" s="24" t="s">
         <v>5</v>
       </c>
@@ -2275,7 +2360,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10">
       <c r="B34" s="45"/>
       <c r="C34" s="46"/>
       <c r="D34" s="47"/>
@@ -2289,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="15.75" thickBot="1">
       <c r="B35" s="28"/>
       <c r="C35" s="29"/>
       <c r="D35" s="30"/>
@@ -2303,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10">
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
       <c r="D36" s="13"/>
@@ -2328,14 +2413,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733C2A37-09AA-41E6-B976-502F90A9005E}">
-  <dimension ref="B1:P23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:P45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1"/>
@@ -2349,15 +2434,15 @@
     <col min="16" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D2" s="54" t="s">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:16">
+      <c r="D2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="55"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="40">
         <f>SUM(J:J)</f>
-        <v>0</v>
+        <v>-4.82</v>
       </c>
       <c r="G2" s="42" t="s">
         <v>2</v>
@@ -2367,25 +2452,25 @@
       </c>
       <c r="I2" s="2">
         <f>COUNTIF(B:B,"YES")</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="60" t="e">
-        <f>SUM(E6:E150)/COUNT(E6:E150)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="56" t="s">
+      <c r="L2" s="55"/>
+      <c r="M2" s="56">
+        <f>SUM(E6:E172)/COUNT(E6:E172)</f>
+        <v>1.2727272727272727</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickBot="1">
+      <c r="D3" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="41" t="e">
+      <c r="E3" s="67"/>
+      <c r="F3" s="41">
         <f>SUM(J:J)/SUM(E:E)*100</f>
-        <v>#DIV/0!</v>
+        <v>-34.428571428571431</v>
       </c>
       <c r="G3" s="43" t="s">
         <v>40</v>
@@ -2395,19 +2480,19 @@
       </c>
       <c r="I3" s="4">
         <f>COUNTIF(B:B,"NO")</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63" t="e">
-        <f>SUM(D6:D150)/COUNT(D6:D150)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="58"/>
+      <c r="M3" s="59">
+        <f>SUM(D6:D172)/COUNT(D6:D172)</f>
+        <v>2.0390909090909091</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1">
       <c r="B5" s="36" t="s">
         <v>9</v>
       </c>
@@ -2436,208 +2521,398 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="35">
-        <f t="shared" ref="J6:J16" si="0">IF(B6="YES",SUM(D6-1)*E6,IF(B6="NO",-E6,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="64" t="s">
+    <row r="6" spans="2:16">
+      <c r="B6" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="62">
+        <v>2</v>
+      </c>
+      <c r="E6" s="62">
+        <v>2</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="63">
+        <f t="shared" ref="J6:J38" si="0">IF(B6="YES",SUM(D6-1)*E6,IF(B6="NO",-E6,0))</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
+      <c r="B7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="62">
+        <v>2.4</v>
+      </c>
+      <c r="E7" s="62">
+        <v>1</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="23">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M7" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-    </row>
-    <row r="9" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B9" s="26"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="66">
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+    </row>
+    <row r="8" spans="2:16">
+      <c r="B8" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="79">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E8" s="79">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" s="81">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+    </row>
+    <row r="9" spans="2:16" ht="28.5">
+      <c r="B9" s="78"/>
+      <c r="C9" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" s="82"/>
+      <c r="M9" s="69">
         <f>F2</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="66"/>
-      <c r="O9" s="65" t="s">
+        <v>-4.82</v>
+      </c>
+      <c r="N9" s="69"/>
+      <c r="O9" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="P9" s="65"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="26"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="26"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="27">
-        <f t="shared" ref="J17:J23" si="1">IF(B17="YES",SUM(D17-1)*E17,IF(B17="NO",-E17,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="P9" s="70"/>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="B10" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="25">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
+      <c r="B11" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="73">
+        <v>2.9</v>
+      </c>
+      <c r="E11" s="73">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="75">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
+      <c r="B12" s="72"/>
+      <c r="C12" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="76"/>
+    </row>
+    <row r="13" spans="2:16">
+      <c r="B13" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1.85</v>
+      </c>
+      <c r="E13" s="11">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="23">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
+      <c r="B14" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1.7</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="25">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
+      <c r="B15" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1.72</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="25">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="B16" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="E16" s="11">
+        <v>2</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" s="23">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="11">
+        <v>2</v>
+      </c>
+      <c r="E17" s="11">
+        <v>2</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" s="23">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1.66</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" s="25">
+        <f t="shared" si="0"/>
+        <v>0.65999999999999992</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
       <c r="B19" s="26"/>
       <c r="C19" s="15"/>
       <c r="D19" s="10"/>
@@ -2647,11 +2922,11 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
       <c r="B20" s="26"/>
       <c r="C20" s="15"/>
       <c r="D20" s="10"/>
@@ -2661,11 +2936,11 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
       <c r="B21" s="26"/>
       <c r="C21" s="15"/>
       <c r="D21" s="10"/>
@@ -2675,11 +2950,11 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
       <c r="B22" s="26"/>
       <c r="C22" s="15"/>
       <c r="D22" s="10"/>
@@ -2689,45 +2964,361 @@
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="26"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="26"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="26"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="26"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="26"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="26"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="26"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="26"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="26"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="26"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="26"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="26"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="26"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="26"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="26"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="26"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="26"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="27">
+        <f t="shared" ref="J39:J45" si="1">IF(B39="YES",SUM(D39-1)*E39,IF(B39="NO",-E39,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="26"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="31">
+    <row r="41" spans="2:10">
+      <c r="B41" s="26"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="26"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" s="26"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="26"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B45" s="28"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="13">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="M7:P8"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="J8:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1"/>
@@ -2741,12 +3332,12 @@
     <col min="16" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D2" s="54" t="s">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:16">
+      <c r="D2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="55"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="40">
         <f>SUM(J:J)</f>
         <v>0</v>
@@ -2761,20 +3352,20 @@
         <f>COUNTIF(B:B,"YES")</f>
         <v>0</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="60" t="e">
+      <c r="L2" s="55"/>
+      <c r="M2" s="56" t="e">
         <f>SUM(E6:E150)/COUNT(E6:E150)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="56" t="s">
+    <row r="3" spans="2:16" ht="15.75" thickBot="1">
+      <c r="D3" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="57"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="41" t="e">
         <f>SUM(J:J)/SUM(E:E)*100</f>
         <v>#DIV/0!</v>
@@ -2789,17 +3380,17 @@
         <f>COUNTIF(B:B,"NO")</f>
         <v>0</v>
       </c>
-      <c r="K3" s="61" t="s">
+      <c r="K3" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63" t="e">
+      <c r="L3" s="58"/>
+      <c r="M3" s="59" t="e">
         <f>SUM(D6:D150)/COUNT(D6:D150)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1">
       <c r="B5" s="36" t="s">
         <v>9</v>
       </c>
@@ -2828,7 +3419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16">
       <c r="B6" s="32"/>
       <c r="C6" s="33"/>
       <c r="D6" s="34"/>
@@ -2842,7 +3433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16">
       <c r="B7" s="26"/>
       <c r="C7" s="15"/>
       <c r="D7" s="10"/>
@@ -2855,14 +3446,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M7" s="64" t="s">
+      <c r="M7" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" s="26"/>
       <c r="C8" s="15"/>
       <c r="D8" s="10"/>
@@ -2875,12 +3466,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-    </row>
-    <row r="9" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+    </row>
+    <row r="9" spans="2:16" ht="28.5">
       <c r="B9" s="26"/>
       <c r="C9" s="15"/>
       <c r="D9" s="10"/>
@@ -2893,17 +3484,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M9" s="66">
+      <c r="M9" s="69">
         <f>F2</f>
         <v>0</v>
       </c>
-      <c r="N9" s="66"/>
-      <c r="O9" s="65" t="s">
+      <c r="N9" s="69"/>
+      <c r="O9" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="P9" s="65"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P9" s="70"/>
+    </row>
+    <row r="10" spans="2:16">
       <c r="B10" s="26"/>
       <c r="C10" s="15"/>
       <c r="D10" s="10"/>
@@ -2917,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16">
       <c r="B11" s="26"/>
       <c r="C11" s="15"/>
       <c r="D11" s="10"/>
@@ -2931,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16">
       <c r="B12" s="26"/>
       <c r="C12" s="15"/>
       <c r="D12" s="10"/>
@@ -2945,7 +3536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16">
       <c r="B13" s="26"/>
       <c r="C13" s="15"/>
       <c r="D13" s="10"/>
@@ -2959,7 +3550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16">
       <c r="B14" s="26"/>
       <c r="C14" s="15"/>
       <c r="D14" s="10"/>
@@ -2973,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16">
       <c r="B15" s="26"/>
       <c r="C15" s="15"/>
       <c r="D15" s="10"/>
@@ -2987,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16">
       <c r="B16" s="26"/>
       <c r="C16" s="15"/>
       <c r="D16" s="10"/>
@@ -3001,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="B17" s="26"/>
       <c r="C17" s="15"/>
       <c r="D17" s="10"/>
@@ -3015,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10">
       <c r="B18" s="26"/>
       <c r="C18" s="15"/>
       <c r="D18" s="10"/>
@@ -3029,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10">
       <c r="B19" s="26"/>
       <c r="C19" s="15"/>
       <c r="D19" s="10"/>
@@ -3043,7 +3634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10">
       <c r="B20" s="26"/>
       <c r="C20" s="15"/>
       <c r="D20" s="10"/>
@@ -3057,7 +3648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10">
       <c r="B21" s="26"/>
       <c r="C21" s="15"/>
       <c r="D21" s="10"/>
@@ -3071,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10">
       <c r="B22" s="26"/>
       <c r="C22" s="15"/>
       <c r="D22" s="10"/>
@@ -3085,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="15.75" thickBot="1">
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
       <c r="D23" s="30"/>

</xml_diff>